<commit_message>
feat : bayesian inference base model
</commit_message>
<xml_diff>
--- a/src/random_forest_feature_importance.xlsx
+++ b/src/random_forest_feature_importance.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2985817045641871</v>
+        <v>0.2991889419943792</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06810401799154617</v>
+        <v>0.06826131483818645</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05436820236923981</v>
+        <v>0.05472762994605947</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03625220919501735</v>
+        <v>0.03627575334464839</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03549484415705961</v>
+        <v>0.03605868920991648</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02838541336667934</v>
+        <v>0.02892735437053113</v>
       </c>
     </row>
     <row r="8">
@@ -512,17 +512,17 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02644304027108038</v>
+        <v>0.02671757396340805</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Country of residence_Nigeria</t>
+          <t>Programming is primarily for individuals with strong mathematical or technical backgrounds</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02118454721053119</v>
+        <v>0.02214951105968853</v>
       </c>
     </row>
     <row r="10">
@@ -532,77 +532,77 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02113123244616489</v>
+        <v>0.02188639950398212</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>How much electricity access do you have to learn programming per day?</t>
+          <t>Country of residence_Nigeria</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0208218672074477</v>
+        <v>0.02162327023633552</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Programming is primarily for individuals with strong mathematical or technical backgrounds</t>
+          <t>Employment status</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02064543083106385</v>
+        <v>0.020813054788948</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Employment status</t>
+          <t>I have encountered societal beliefs that discourage my pursuit of computer programming</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01987741375326102</v>
+        <v>0.01995918008489123</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>I have encountered societal beliefs that discourage my pursuit of computer programming</t>
+          <t>It is important for me to see more representation of my cultural or societal background in the programming industry</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01864180204914266</v>
+        <v>0.01824195851240663</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>It is important for me to see more representation of my cultural or societal background in the programming industry</t>
+          <t>My immediate family is supportive of my decision to pursue programming</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01752094992862836</v>
+        <v>0.01811134141549349</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>My immediate family is supportive of my decision to pursue programming</t>
+          <t>I have experienced societal pressure to pursue traditional career paths instead of programming</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01686887379918778</v>
+        <v>0.01777049485263905</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>I have experienced societal pressure to pursue traditional career paths instead of programming</t>
+          <t>I have faced gender-related barriers or stereotypes that discourage my involvement in programming</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01685150938718023</v>
+        <v>0.01674723479807783</v>
       </c>
     </row>
     <row r="18">
@@ -612,37 +612,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01650132407004639</v>
+        <v>0.01665973270505237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>I have faced gender-related barriers or stereotypes that discourage my involvement in programming</t>
+          <t>It is important for me to have access to mentors or role models in the field of computer programming</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.01575169336084991</v>
+        <v>0.01564709726321841</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>It is important for me to have access to mentors or role models in the field of computer programming</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01525413080468876</v>
+        <v>0.01537291076540824</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Do you have access to a computer or laptop at your home or within your community?</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.01473433071071267</v>
+        <v>0.01364846303272846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>